<commit_message>
Update evaluation grid 2
</commit_message>
<xml_diff>
--- a/conception/Grille dévaluation Projet Java-Uml-POO.xlsx
+++ b/conception/Grille dévaluation Projet Java-Uml-POO.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julien\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Etienne\Desktop\JavaProject\JavaProject_Boulderdash\conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="13905" windowHeight="8370"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="13905" windowHeight="8370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Projet" sheetId="1" r:id="rId1"/>
     <sheet name="Cahier de test" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1331,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2438,8 +2438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="B1" s="49" t="str">
         <f>B3</f>
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -2469,14 +2469,14 @@
       </c>
       <c r="B3" s="12" t="str">
         <f>IF(D3&gt;16,"A",IF(D3&gt;10.5,"B",IF(D3&gt;5.5,"C","D")))</f>
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="12">
         <f>SUM(D4:D13)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>3</v>
@@ -2486,7 +2486,9 @@
       <c r="A4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="16">
+        <v>0</v>
+      </c>
       <c r="C4" s="5">
         <v>3</v>
       </c>
@@ -2502,13 +2504,15 @@
       <c r="A5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="17"/>
+      <c r="B5" s="17">
+        <v>1</v>
+      </c>
       <c r="C5" s="6">
         <v>3</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ref="D5:D13" si="0">(B5/E5)*C5</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E5" s="6">
         <v>2</v>
@@ -2518,13 +2522,15 @@
       <c r="A6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="17">
+        <v>2</v>
+      </c>
       <c r="C6" s="6">
         <v>3</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E6" s="6">
         <v>2</v>
@@ -2534,7 +2540,9 @@
       <c r="A7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="17">
+        <v>0</v>
+      </c>
       <c r="C7" s="6">
         <v>2</v>
       </c>
@@ -2550,13 +2558,15 @@
       <c r="A8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="17">
+        <v>1</v>
+      </c>
       <c r="C8" s="6">
         <v>2</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="6">
         <v>1</v>
@@ -2566,7 +2576,9 @@
       <c r="A9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="17"/>
+      <c r="B9" s="17">
+        <v>0</v>
+      </c>
       <c r="C9" s="6">
         <v>2</v>
       </c>
@@ -2582,7 +2594,9 @@
       <c r="A10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="17"/>
+      <c r="B10" s="17">
+        <v>0</v>
+      </c>
       <c r="C10" s="6">
         <v>2</v>
       </c>
@@ -2598,13 +2612,15 @@
       <c r="A11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="17"/>
+      <c r="B11" s="17">
+        <v>1</v>
+      </c>
       <c r="C11" s="6">
         <v>3</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E11" s="6">
         <v>2</v>
@@ -2614,13 +2630,15 @@
       <c r="A12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="17">
+        <v>1</v>
+      </c>
       <c r="C12" s="6">
         <v>1</v>
       </c>
       <c r="D12" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="6">
         <v>1</v>
@@ -2630,7 +2648,9 @@
       <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="18"/>
+      <c r="B13" s="18">
+        <v>0</v>
+      </c>
       <c r="C13" s="7">
         <v>1</v>
       </c>

</xml_diff>